<commit_message>
Renamed perClass images from common names to species names
</commit_message>
<xml_diff>
--- a/Museum_indoors_big.xlsx
+++ b/Museum_indoors_big.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\batra\Documents\Emily Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\proto\OneDrive\Documents\Emily_Capstone\Museum_spec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC25D9F3-F0DE-450A-AF7A-96E858458DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA456F7D-388D-4E51-8FC9-AD0A7E6B410C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Objects" sheetId="1" r:id="rId1"/>
@@ -94,9 +94,6 @@
     <t>Standard deviation</t>
   </si>
   <si>
-    <t>lorikeet_ventral_3_2024-08-05_11-36-35</t>
-  </si>
-  <si>
     <t>throat</t>
   </si>
   <si>
@@ -115,16 +112,10 @@
     <t>yellow_breast2</t>
   </si>
   <si>
-    <t>lorikeet_dorsal_4_2024-08-05_11-37-04</t>
-  </si>
-  <si>
     <t>head</t>
   </si>
   <si>
     <t>back</t>
-  </si>
-  <si>
-    <t>turacoe_dorsal_6_2024-08-05_11-38-44</t>
   </si>
   <si>
     <t>wings_1</t>
@@ -136,16 +127,10 @@
     <t>wings_3</t>
   </si>
   <si>
-    <t>monal_dorsal_1_8_2024-08-05_11-41-57</t>
-  </si>
-  <si>
     <t>mantle1</t>
   </si>
   <si>
     <t>mantle2</t>
-  </si>
-  <si>
-    <t>monal_dorsal_2_9_2024-08-05_11-42-44</t>
   </si>
   <si>
     <t>bottom_back</t>
@@ -155,9 +140,6 @@
   </si>
   <si>
     <t>purple_section2</t>
-  </si>
-  <si>
-    <t>gallus_dorsal_10_2024-08-05_11-44-22</t>
   </si>
   <si>
     <t>throat_light</t>
@@ -178,19 +160,10 @@
     <t>belly_full</t>
   </si>
   <si>
-    <t>raven_ventral_12_2024-08-05_11-46-04</t>
-  </si>
-  <si>
     <t>belly</t>
   </si>
   <si>
-    <t>quail_ventral_14_2024-08-05_11-47-55</t>
-  </si>
-  <si>
     <t>ventral_gray</t>
-  </si>
-  <si>
-    <t>quail_dorsal_15_2024-08-05_11-48-27</t>
   </si>
   <si>
     <t>nape_light</t>
@@ -214,12 +187,6 @@
     <t>purple_belly_full</t>
   </si>
   <si>
-    <t>poorwill_ventral_18_2024-08-05_11-51-52</t>
-  </si>
-  <si>
-    <t>poorwill_dorsal_19_2024-08-05_11-52-22</t>
-  </si>
-  <si>
     <t>back_light</t>
   </si>
   <si>
@@ -232,16 +199,49 @@
     <t>back_full</t>
   </si>
   <si>
-    <t>blackbird_ventral_20_2024-08-05_11-54-52</t>
+    <t>Corvus.corax_ventral_12_2024-08-05_11-46-04</t>
   </si>
   <si>
-    <t>stellars.jay_ventral_13_2024-08-05_11-46-58</t>
+    <t>Euphagus.carolinus_ventral_20_2024-08-05_11-54-52</t>
   </si>
   <si>
-    <t>splendid.starling_ventral_16_2024-08-05_11-49-29</t>
+    <t>Gallus.sonneratii_dorsal_10_2024-08-05_11-44-22</t>
   </si>
   <si>
-    <t>european.starling_ventral_17_2024-08-05_11-50-23</t>
+    <t>Lophoporus.impeyanus_dorsal_1_8_2024-08-05_11-41-57</t>
+  </si>
+  <si>
+    <t>Lophoporus.impeyanus_dorsal_2_9_2024-08-05_11-42-44</t>
+  </si>
+  <si>
+    <t>Callipepla.californica_ventral_14_2024-08-05_11-47-55</t>
+  </si>
+  <si>
+    <t>Callipepla.californica_dorsal_15_2024-08-05_11-48-27</t>
+  </si>
+  <si>
+    <t>Phalaenoptilus.nuttallii_ventral_18_2024-08-05_11-51-52</t>
+  </si>
+  <si>
+    <t>Phalaenoptilus.nuttallii_dorsal_19_2024-08-05_11-52-22</t>
+  </si>
+  <si>
+    <t>Cyanocitta.stelleri_ventral_13_2024-08-05_11-46-58</t>
+  </si>
+  <si>
+    <t>Sturnus.vulgaris_ventral_17_2024-08-05_11-50-23</t>
+  </si>
+  <si>
+    <t>Lamprotornis.splendidus_ventral_16_2024-08-05_11-49-29</t>
+  </si>
+  <si>
+    <t>Tauraco.harlaubi_dorsal_6_2024-08-05_11-38-44</t>
+  </si>
+  <si>
+    <t>Trichoglossus.moluccanus_ventral_3_2024-08-05_11-36-35</t>
+  </si>
+  <si>
+    <t>Trichoglossus.moluccanus_dorsal_4_2024-08-05_11-37-04</t>
   </si>
 </sst>
 </file>
@@ -612,16 +612,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:MB53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.140625" customWidth="1"/>
+    <col min="1" max="1" width="40.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -635,7 +635,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -646,7 +646,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:340" x14ac:dyDescent="0.3">
       <c r="L4" t="s">
         <v>20</v>
       </c>
@@ -654,7 +654,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2680,12 +2680,12 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="7" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
       </c>
       <c r="C7">
         <v>221</v>
@@ -2700,7 +2700,7 @@
         <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -3693,12 +3693,12 @@
         <v>5.8096889406442642E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>215</v>
@@ -3713,7 +3713,7 @@
         <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -4706,12 +4706,12 @@
         <v>0.10264752805233002</v>
       </c>
     </row>
-    <row r="9" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9">
         <v>217</v>
@@ -4726,7 +4726,7 @@
         <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -5719,12 +5719,12 @@
         <v>8.3111897110939026E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>193</v>
@@ -5739,7 +5739,7 @@
         <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -6732,12 +6732,12 @@
         <v>6.7249514162540436E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>277</v>
@@ -6752,7 +6752,7 @@
         <v>26</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -7745,12 +7745,12 @@
         <v>7.1841277182102203E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>227</v>
@@ -7765,7 +7765,7 @@
         <v>58</v>
       </c>
       <c r="G12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -8758,12 +8758,12 @@
         <v>0.15483072400093079</v>
       </c>
     </row>
-    <row r="13" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" t="s">
         <v>31</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
       </c>
       <c r="C13">
         <v>203</v>
@@ -8778,7 +8778,7 @@
         <v>123</v>
       </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
@@ -9771,12 +9771,12 @@
         <v>7.8256800770759583E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C14">
         <v>190</v>
@@ -9791,7 +9791,7 @@
         <v>113</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
@@ -10784,12 +10784,12 @@
         <v>6.8487823009490967E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>255</v>
@@ -10804,7 +10804,7 @@
         <v>69</v>
       </c>
       <c r="G15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
@@ -11797,12 +11797,12 @@
         <v>4.413478821516037E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C16">
         <v>189</v>
@@ -11817,7 +11817,7 @@
         <v>39</v>
       </c>
       <c r="G16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -12810,12 +12810,12 @@
         <v>3.9997149258852005E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" t="s">
         <v>34</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
       </c>
       <c r="C17">
         <v>174</v>
@@ -12830,7 +12830,7 @@
         <v>38</v>
       </c>
       <c r="G17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I17" t="b">
         <v>1</v>
@@ -13823,12 +13823,12 @@
         <v>4.6930298209190369E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>155</v>
@@ -13843,7 +13843,7 @@
         <v>34</v>
       </c>
       <c r="G18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I18" t="b">
         <v>1</v>
@@ -14836,12 +14836,12 @@
         <v>6.2817074358463287E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C19">
         <v>91</v>
@@ -14856,7 +14856,7 @@
         <v>59</v>
       </c>
       <c r="G19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
@@ -15849,12 +15849,12 @@
         <v>4.5336727052927017E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C20">
         <v>106</v>
@@ -15869,7 +15869,7 @@
         <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I20" t="b">
         <v>1</v>
@@ -16862,12 +16862,12 @@
         <v>7.5638800859451294E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C21">
         <v>66</v>
@@ -16882,7 +16882,7 @@
         <v>122</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I21" t="b">
         <v>1</v>
@@ -17875,12 +17875,12 @@
         <v>5.0402544438838959E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C22">
         <v>71</v>
@@ -17895,7 +17895,7 @@
         <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
@@ -18888,12 +18888,12 @@
         <v>0.29676362872123718</v>
       </c>
     </row>
-    <row r="23" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C23">
         <v>325</v>
@@ -18908,7 +18908,7 @@
         <v>18</v>
       </c>
       <c r="G23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I23" t="b">
         <v>1</v>
@@ -19901,12 +19901,12 @@
         <v>0.41752517223358154</v>
       </c>
     </row>
-    <row r="24" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C24">
         <v>210</v>
@@ -19921,7 +19921,7 @@
         <v>4</v>
       </c>
       <c r="G24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I24" t="b">
         <v>1</v>
@@ -20914,12 +20914,12 @@
         <v>0.11636763066053391</v>
       </c>
     </row>
-    <row r="25" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C25">
         <v>196</v>
@@ -20934,7 +20934,7 @@
         <v>4</v>
       </c>
       <c r="G25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -21927,12 +21927,12 @@
         <v>3.957231342792511E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C26">
         <v>112</v>
@@ -21947,7 +21947,7 @@
         <v>119</v>
       </c>
       <c r="G26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I26" t="b">
         <v>1</v>
@@ -22940,12 +22940,12 @@
         <v>0.19031175971031189</v>
       </c>
     </row>
-    <row r="27" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C27">
         <v>268</v>
@@ -22960,7 +22960,7 @@
         <v>7</v>
       </c>
       <c r="G27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I27" t="b">
         <v>1</v>
@@ -23953,12 +23953,12 @@
         <v>4.2184818536043167E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C28">
         <v>256</v>
@@ -23973,7 +23973,7 @@
         <v>8</v>
       </c>
       <c r="G28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I28" t="b">
         <v>1</v>
@@ -24966,12 +24966,12 @@
         <v>2.0992191508412361E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" t="s">
         <v>45</v>
-      </c>
-      <c r="B29" t="s">
-        <v>51</v>
       </c>
       <c r="C29">
         <v>148</v>
@@ -24986,7 +24986,7 @@
         <v>116</v>
       </c>
       <c r="G29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -25979,12 +25979,12 @@
         <v>4.1309770196676254E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C30">
         <v>173</v>
@@ -25999,7 +25999,7 @@
         <v>38</v>
       </c>
       <c r="G30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I30" t="b">
         <v>1</v>
@@ -26992,12 +26992,12 @@
         <v>6.4099743962287903E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C31">
         <v>178</v>
@@ -27012,7 +27012,7 @@
         <v>79</v>
       </c>
       <c r="G31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I31" t="b">
         <v>1</v>
@@ -28005,12 +28005,12 @@
         <v>9.4102993607521057E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C32">
         <v>184</v>
@@ -28025,7 +28025,7 @@
         <v>47</v>
       </c>
       <c r="G32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I32" t="b">
         <v>1</v>
@@ -29018,12 +29018,12 @@
         <v>6.0012299567461014E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C33">
         <v>243</v>
@@ -29038,7 +29038,7 @@
         <v>7</v>
       </c>
       <c r="G33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
@@ -30031,12 +30031,12 @@
         <v>6.2821991741657257E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C34">
         <v>222</v>
@@ -30051,7 +30051,7 @@
         <v>4</v>
       </c>
       <c r="G34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I34" t="b">
         <v>1</v>
@@ -31044,12 +31044,12 @@
         <v>1.9152157008647919E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C35">
         <v>185</v>
@@ -31064,7 +31064,7 @@
         <v>104</v>
       </c>
       <c r="G35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I35" t="b">
         <v>1</v>
@@ -32057,12 +32057,12 @@
         <v>0.22671608626842499</v>
       </c>
     </row>
-    <row r="36" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C36">
         <v>241</v>
@@ -32077,7 +32077,7 @@
         <v>4</v>
       </c>
       <c r="G36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I36" t="b">
         <v>1</v>
@@ -33070,12 +33070,12 @@
         <v>1.3182315044105053E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C37">
         <v>262</v>
@@ -33090,7 +33090,7 @@
         <v>3</v>
       </c>
       <c r="G37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I37" t="b">
         <v>1</v>
@@ -34083,12 +34083,12 @@
         <v>6.3933557830750942E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C38">
         <v>229</v>
@@ -34103,7 +34103,7 @@
         <v>16</v>
       </c>
       <c r="G38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I38" t="b">
         <v>1</v>
@@ -35096,12 +35096,12 @@
         <v>3.4729521721601486E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C39">
         <v>209</v>
@@ -35116,7 +35116,7 @@
         <v>14</v>
       </c>
       <c r="G39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I39" t="b">
         <v>1</v>
@@ -36109,12 +36109,12 @@
         <v>6.4974218606948853E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C40">
         <v>255</v>
@@ -36129,7 +36129,7 @@
         <v>8</v>
       </c>
       <c r="G40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I40" t="b">
         <v>1</v>
@@ -37122,12 +37122,12 @@
         <v>9.9600683897733688E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B41" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C41">
         <v>225</v>
@@ -37142,7 +37142,7 @@
         <v>6</v>
       </c>
       <c r="G41" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I41" t="b">
         <v>1</v>
@@ -38135,12 +38135,12 @@
         <v>1.3212818652391434E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B42" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C42">
         <v>225</v>
@@ -38155,7 +38155,7 @@
         <v>17</v>
       </c>
       <c r="G42" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I42" t="b">
         <v>1</v>
@@ -39148,12 +39148,12 @@
         <v>3.8250111043453217E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C43">
         <v>236</v>
@@ -39168,7 +39168,7 @@
         <v>5</v>
       </c>
       <c r="G43" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I43" t="b">
         <v>1</v>
@@ -40161,12 +40161,12 @@
         <v>3.823871910572052E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C44">
         <v>226</v>
@@ -40181,7 +40181,7 @@
         <v>5</v>
       </c>
       <c r="G44" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I44" t="b">
         <v>1</v>
@@ -41174,12 +41174,12 @@
         <v>2.540653757750988E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C45">
         <v>202</v>
@@ -41194,7 +41194,7 @@
         <v>105</v>
       </c>
       <c r="G45" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I45" t="b">
         <v>1</v>
@@ -42187,12 +42187,12 @@
         <v>0.22116671502590179</v>
       </c>
     </row>
-    <row r="46" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B46" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C46">
         <v>265</v>
@@ -42207,7 +42207,7 @@
         <v>5</v>
       </c>
       <c r="G46" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I46" t="b">
         <v>1</v>
@@ -43200,12 +43200,12 @@
         <v>4.9457985907793045E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C47">
         <v>252</v>
@@ -43220,7 +43220,7 @@
         <v>6</v>
       </c>
       <c r="G47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I47" t="b">
         <v>1</v>
@@ -44213,12 +44213,12 @@
         <v>6.6441893577575684E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C48">
         <v>214</v>
@@ -44233,7 +44233,7 @@
         <v>57</v>
       </c>
       <c r="G48" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I48" t="b">
         <v>1</v>
@@ -45226,12 +45226,12 @@
         <v>0.19759377837181091</v>
       </c>
     </row>
-    <row r="49" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C49">
         <v>212</v>
@@ -45246,7 +45246,7 @@
         <v>4</v>
       </c>
       <c r="G49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I49" t="b">
         <v>1</v>
@@ -46239,12 +46239,12 @@
         <v>3.6695115268230438E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B50" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C50">
         <v>246</v>
@@ -46259,7 +46259,7 @@
         <v>6</v>
       </c>
       <c r="G50" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I50" t="b">
         <v>1</v>
@@ -47252,12 +47252,12 @@
         <v>6.2797978520393372E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B51" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C51">
         <v>196</v>
@@ -47272,7 +47272,7 @@
         <v>6</v>
       </c>
       <c r="G51" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I51" t="b">
         <v>1</v>
@@ -48265,12 +48265,12 @@
         <v>5.9063751250505447E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B52" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C52">
         <v>194</v>
@@ -48285,7 +48285,7 @@
         <v>109</v>
       </c>
       <c r="G52" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I52" t="b">
         <v>1</v>
@@ -49278,12 +49278,12 @@
         <v>0.13088783621788025</v>
       </c>
     </row>
-    <row r="53" spans="1:340" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:340" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C53">
         <v>190</v>
@@ -49298,7 +49298,7 @@
         <v>31</v>
       </c>
       <c r="G53" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I53" t="b">
         <v>1</v>

</xml_diff>